<commit_message>
xong toan bo chuc nang co ban
</commit_message>
<xml_diff>
--- a/ketquadongdoi.xlsx
+++ b/ketquadongdoi.xlsx
@@ -71,7 +71,19 @@
     <t xml:space="preserve">HCM 3</t>
   </si>
   <si>
-    <t xml:space="preserve">HẠNG 2 ĐỘI: Hà Nội</t>
+    <t xml:space="preserve">HẠNG 2 ĐỘI: QDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QDO 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QDO 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 3 ĐỘI: Hà Nội</t>
   </si>
   <si>
     <t xml:space="preserve">Hà Nội 1</t>
@@ -81,18 +93,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hà Nội 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 3 ĐỘI: QDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO 2</t>
   </si>
   <si>
     <t xml:space="preserve">HẠNG 4 ĐỘI: THO</t>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s" s="11">
         <v>13</v>
@@ -1550,21 +1550,21 @@
         <v>14</v>
       </c>
       <c r="D7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F7" s="8">
         <v>10</v>
       </c>
       <c r="G7" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s" s="11">
         <v>15</v>
@@ -1573,10 +1573,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s" s="11">
         <v>17</v>
@@ -1603,21 +1603,21 @@
         <v>18</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F10" s="8">
         <v>10</v>
       </c>
       <c r="G10" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s" s="11">
         <v>19</v>
@@ -1626,10 +1626,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>

</xml_diff>

<commit_message>
hoan thanh ung dung tinh hang dong doi
</commit_message>
<xml_diff>
--- a/ketquadongdoi.xlsx
+++ b/ketquadongdoi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lap Trinh\NodeJs\BocThamVongTron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D69057-68D6-4BE9-9DEE-136921D96410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2109AE12-39B2-487E-AFBF-0D802E99E6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>Đơn Vị</t>
   </si>
   <si>
-    <t>Điểm Số</t>
-  </si>
-  <si>
     <t>Tổng Hạng</t>
   </si>
   <si>
@@ -59,91 +56,127 @@
     <t>XẾP HẠNG ĐỒNG ĐỘI</t>
   </si>
   <si>
-    <t xml:space="preserve">HẠNG 1 ĐỘI: HCM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCM 4</t>
+    <t>Điểm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 1 ĐỘI: NAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngô Hùng Phương</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngô Minh Huấn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 2 ĐỘI: VTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vũ Lương Minh Đức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phạm Tuấn Kiệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 3 ĐỘI: THO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Bá Nguyên Lâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đỗ Thị Ngọc Anh (Nữ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 4 ĐỘI: DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Đức Cường</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Đức Quang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 5 ĐỘI: CTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đỗ Bảo Hân (Nữ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàng Thùy Dương (Nữ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 6 ĐỘI: QDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàng Đình Bảo Duy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Hải Vân (Nữ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 7 ĐỘI: KGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàng Trường Giang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Nguyên Bảo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 8 ĐỘI: BTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Tùng Minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phạm Xuân Phúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 9 ĐỘI: HCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vũ Nguyễn Nguyên Khang</t>
   </si>
   <si>
     <t xml:space="preserve">HCM</t>
   </si>
   <si>
-    <t xml:space="preserve">HCM 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 2 ĐỘI: QDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 3 ĐỘI: Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hà Nội 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hà Nội 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 4 ĐỘI: THO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thanh Hóa 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 5 ĐỘI: BNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hà Nội 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 6 ĐỘI: QNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCM 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 7 ĐỘI: TBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 8 ĐỘI: BTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QDO 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HẠNG 9 ĐỘI: LCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCA</t>
+    <t xml:space="preserve">Hoàng Dũng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 10 ĐỘI: HNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Đắc Cao Phong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Thế Hiệp</t>
   </si>
 </sst>
 </file>
@@ -160,23 +193,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -228,35 +266,35 @@
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1426,945 +1464,1016 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="5.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="9">
+      <c r="A1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="7">
+      <c r="F2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s" s="6">
+      <c r="E4" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s" s="11">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8">
-        <v>5</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4</v>
+      <c r="E5" s="6">
+        <v>5.5</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="10">
+    <row r="6" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s" s="11">
+      <c r="A7" s="6">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7</v>
+      </c>
+      <c r="F7" s="8">
         <v>8</v>
       </c>
-      <c r="F7" s="8">
-        <v>10</v>
-      </c>
       <c r="G7" s="8">
-        <v>12</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s" s="11">
+      <c r="A8" s="6">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="C8" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="6">
         <v>7</v>
       </c>
-      <c r="E8" s="2">
-        <v>4</v>
+      <c r="E8" s="6">
+        <v>5.5</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="10">
+    <row r="9" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s" s="11">
+      <c r="A10" s="6">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="C10" t="s" s="2">
+      <c r="C10" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D10" s="2">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>6</v>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>5.5</v>
       </c>
       <c r="F10" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G10" s="8">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3</v>
+      <c r="E11" s="6">
+        <v>5</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="10">
+    <row r="12" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="6">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F13" s="8">
         <v>16</v>
       </c>
-      <c r="B13" t="s" s="11">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s" s="2">
+      <c r="G13" s="8">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="D13" s="2">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2">
-        <v>4</v>
-      </c>
-      <c r="F13" s="8">
-        <v>17</v>
-      </c>
-      <c r="G13" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s" s="11">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="D14" s="6">
         <v>11</v>
       </c>
-      <c r="E14" s="2">
-        <v>3</v>
+      <c r="E14" s="6">
+        <v>5</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+    <row r="15" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s" s="11">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s" s="2">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="D16" s="2">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
+      <c r="C16" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="D16" s="6">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6">
+        <v>5.5</v>
       </c>
       <c r="F16" s="8">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G16" s="8">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="D17" s="6">
+        <v>10</v>
+      </c>
+      <c r="E17" s="6">
         <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s" s="11">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="D17" s="2">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+    <row r="18" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A18" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s" s="11">
+      <c r="A19" s="6">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="D19" s="6">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8">
         <v>27</v>
       </c>
-      <c r="C19" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="8">
-        <v>34</v>
-      </c>
       <c r="G19" s="8">
-        <v>3</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2">
-        <v>18</v>
-      </c>
-      <c r="E20" s="2">
-        <v>2</v>
+      <c r="A20" s="6">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6">
+        <v>19</v>
+      </c>
+      <c r="E20" s="6">
+        <v>4.5</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+    <row r="21" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A21" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s" s="11">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s" s="2">
+      <c r="A22" s="6">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="D22" s="6">
+        <v>15</v>
+      </c>
+      <c r="E22" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F22" s="8">
         <v>31</v>
       </c>
-      <c r="D22" s="2">
-        <v>12</v>
-      </c>
-      <c r="E22" s="2">
-        <v>3</v>
-      </c>
-      <c r="F22" s="8">
-        <v>39</v>
-      </c>
       <c r="G22" s="8">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s" s="11">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2">
-        <v>27</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
+      <c r="A23" s="6">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="D23" s="6">
+        <v>16</v>
+      </c>
+      <c r="E23" s="6">
+        <v>4.5</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+    <row r="24" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s" s="11">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D25" s="2">
-        <v>20</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
+      <c r="A25" s="6">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="D25" s="6">
+        <v>23</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4.5</v>
       </c>
       <c r="F25" s="8">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G25" s="8">
-        <v>3</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s" s="11">
+      <c r="A26" s="6">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="D26" s="6">
         <v>34</v>
       </c>
-      <c r="C26" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D26" s="2">
-        <v>21</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
+      <c r="E26" s="6">
+        <v>4</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+    <row r="27" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+      <c r="A28" s="6">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s" s="6">
+        <v>42</v>
+      </c>
+      <c r="D28" s="6">
+        <v>12</v>
+      </c>
+      <c r="E28" s="6">
         <v>5</v>
       </c>
-      <c r="B28" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D28" s="2">
-        <v>28</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2</v>
-      </c>
       <c r="F28" s="8">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="G28" s="8">
-        <v>4</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D29" s="2">
-        <v>31</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2</v>
+      <c r="A29" s="6">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s" s="6">
+        <v>42</v>
+      </c>
+      <c r="D29" s="6">
+        <v>62</v>
+      </c>
+      <c r="E29" s="6">
+        <v>3.5</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+    <row r="30" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
+      <c r="A31" s="6">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="D31" s="6">
+        <v>35</v>
+      </c>
+      <c r="E31" s="6">
+        <v>4</v>
+      </c>
+      <c r="F31" s="8">
+        <v>77</v>
+      </c>
+      <c r="G31" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="A32" s="6">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s" s="6">
+        <v>46</v>
+      </c>
+      <c r="D32" s="6">
+        <v>42</v>
+      </c>
+      <c r="E32" s="6">
+        <v>4</v>
+      </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+    <row r="33" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+    <row r="36" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
+    <row r="39" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+    <row r="42" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+    <row r="45" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
+    <row r="48" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
+    <row r="51" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
+    <row r="54" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
+    <row r="57" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="A58" s="6"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+    <row r="60" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="A61" s="6"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
+    <row r="63" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="2"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
+    <row r="66" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="2"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
+      <c r="A68" s="6"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
+    <row r="69" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="2"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="2"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
+    <row r="72" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="2"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="2"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="F43:F44"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A66:G66"/>
@@ -2381,57 +2490,12 @@
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="A57:G57"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
   </mergeCells>
   <conditionalFormatting sqref="A4">
     <cfRule type="expression" dxfId="48" priority="37">

</xml_diff>

<commit_message>
fix loi 1 nguoi va nhap so
</commit_message>
<xml_diff>
--- a/ketquadongdoi.xlsx
+++ b/ketquadongdoi.xlsx
@@ -57,6 +57,102 @@
   </si>
   <si>
     <t>Điểm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 1 ĐỘI: DHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Vũ An Nhiên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phan Văn Gia Vũ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 2 ĐỘI: GLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạ Nguyễn Thiện Nhân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Đức Duy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 3 ĐỘI: DKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Phúc Minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Bảo Nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 4 ĐỘI: HLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Tiến Hà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Việt Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 5 ĐỘI: CLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Thị Kim Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huỳnh Phúc Lâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 6 ĐỘI: HHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hồ Nguyễn Vân Chi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Tùng Lâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 7 ĐỘI: TPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phạm Ngọc Dũng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hồ Hùng Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 8 ĐỘI: VLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Đức Cao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Bảo Tín</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1490,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
+      <c r="A3" t="s" s="5">
+        <v>8</v>
+      </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1403,25 +1501,51 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="A4" s="6">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="6">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4.5</v>
+      </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
+      <c r="A6" t="s" s="5">
+        <v>12</v>
+      </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1430,25 +1554,51 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="6">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="6">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6">
+        <v>4</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+      <c r="A9" t="s" s="5">
+        <v>16</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1457,25 +1607,51 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="A10" s="6">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="8">
+        <v>13</v>
+      </c>
+      <c r="G10" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="6">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3.5</v>
+      </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
+      <c r="A12" t="s" s="5">
+        <v>20</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1484,25 +1660,51 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="A13" s="6">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4</v>
+      </c>
+      <c r="F13" s="8">
+        <v>15</v>
+      </c>
+      <c r="G13" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="6">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
+      <c r="A15" t="s" s="5">
+        <v>24</v>
+      </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1511,25 +1713,51 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="6">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F16" s="8">
+        <v>16</v>
+      </c>
+      <c r="G16" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="6">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="D17" s="6">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3.5</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
+      <c r="A18" t="s" s="5">
+        <v>28</v>
+      </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1538,25 +1766,51 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="6">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="D19" s="6">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="F19" s="8">
+        <v>28</v>
+      </c>
+      <c r="G19" s="8">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="6">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6">
+        <v>16</v>
+      </c>
+      <c r="E20" s="6">
+        <v>3</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
+      <c r="A21" t="s" s="5">
+        <v>32</v>
+      </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1565,25 +1819,51 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="6">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="D22" s="6">
+        <v>13</v>
+      </c>
+      <c r="E22" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="F22" s="8">
+        <v>28</v>
+      </c>
+      <c r="G22" s="8">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="6">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s" s="6">
+        <v>34</v>
+      </c>
+      <c r="D23" s="6">
+        <v>15</v>
+      </c>
+      <c r="E23" s="6">
+        <v>3</v>
+      </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
+      <c r="A24" t="s" s="5">
+        <v>36</v>
+      </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1592,20 +1872,44 @@
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="6">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="D25" s="6">
+        <v>17</v>
+      </c>
+      <c r="E25" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="F25" s="8">
+        <v>35</v>
+      </c>
+      <c r="G25" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="6">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="D26" s="6">
+        <v>18</v>
+      </c>
+      <c r="E26" s="6">
+        <v>2.5</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>

</xml_diff>

<commit_message>
viet xong phần tổng quát dùng chung chỉ số
</commit_message>
<xml_diff>
--- a/ketquadongdoi.xlsx
+++ b/ketquadongdoi.xlsx
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t xml:space="preserve">Lê Bảo Tín</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HẠNG 9 ĐỘI: TXQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Ngọc Đăng Khoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXQ</t>
   </si>
 </sst>
 </file>
@@ -1567,13 +1576,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="6">
-        <v>10</v>
+        <v>5.5</v>
       </c>
       <c r="F7" s="8">
         <v>7</v>
       </c>
       <c r="G7" s="8">
-        <v>14</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1914,7 +1923,9 @@
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
+      <c r="A27" t="s" s="5">
+        <v>40</v>
+      </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1923,20 +1934,44 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="6">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s" s="6">
+        <v>42</v>
+      </c>
+      <c r="D28" s="6">
+        <v>9</v>
+      </c>
+      <c r="E28" s="6">
+        <v>4</v>
+      </c>
+      <c r="F28" s="8">
+        <v>37</v>
+      </c>
+      <c r="G28" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="6">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s" s="6">
+        <v>42</v>
+      </c>
+      <c r="D29" s="6">
+        <v>28</v>
+      </c>
+      <c r="E29" s="6">
+        <v>4</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>

</xml_diff>